<commit_message>
KETI add RSU model
</commit_message>
<xml_diff>
--- a/docs/naming/5G-NR-V2X_Naming Rule.xlsx
+++ b/docs/naming/5G-NR-V2X_Naming Rule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\내 드라이브\5G-NR-V2X\3차년도\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\work\athena\docs\naming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A807E-2DBE-4919-A559-662DDBE438FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30963C73-83AD-4986-A630-4FC418B5BC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27280" yWindow="490" windowWidth="25920" windowHeight="16010" activeTab="1" xr2:uid="{DDA94870-1869-40B4-BC98-288FA66C3577}"/>
+    <workbookView xWindow="12310" yWindow="7340" windowWidth="23040" windowHeight="12060" activeTab="1" xr2:uid="{DDA94870-1869-40B4-BC98-288FA66C3577}"/>
   </bookViews>
   <sheets>
     <sheet name="Naming Rule" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,10 +141,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>U-CO1XG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NO-CO1XG</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -173,10 +169,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UBUNTU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NVIDIA Orin RxAnt.1 Modem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,6 +186,46 @@
   </si>
   <si>
     <t>Xilinx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>• D : Daebo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>• RG : RSU GPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>• I : Intel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>• XGR : Xsens GPS ROS (RTK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO-CO2XGR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVIDIA Orin RxAnt.2 Modem ROS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI-CO1XG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI-DR2RG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu Intel RSU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu Intel OBU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -347,28 +379,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1014512-47C3-4512-A923-4E33A01C8EE0}">
-  <dimension ref="B2:S12"/>
+  <dimension ref="B2:S13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -723,7 +755,7 @@
   <sheetData>
     <row r="2" spans="2:19" ht="23" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -749,17 +781,17 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.45">
       <c r="C4" s="2"/>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="3"/>
@@ -767,40 +799,40 @@
         <v>21</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="11" t="s">
+      <c r="M4" s="10"/>
+      <c r="N4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q4" s="3"/>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.45">
       <c r="C5" s="2"/>
-      <c r="D5" s="11"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="11"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="3"/>
       <c r="J5" s="13"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="11"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="11"/>
+      <c r="P5" s="9"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="11"/>
+      <c r="R5" s="9"/>
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="2:19" ht="9" customHeight="1" x14ac:dyDescent="0.45">
@@ -853,6 +885,9 @@
       <c r="F9" t="s">
         <v>4</v>
       </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
@@ -870,14 +905,27 @@
       <c r="F10" t="s">
         <v>5</v>
       </c>
+      <c r="N10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="L12" s="7" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="L13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -896,7 +944,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M12" r:id="rId1" xr:uid="{89252D60-EFB0-4C24-8A7A-CCB272DC6C33}"/>
+    <hyperlink ref="M13" r:id="rId1" xr:uid="{89252D60-EFB0-4C24-8A7A-CCB272DC6C33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -908,7 +956,7 @@
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -928,136 +976,144 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C17" s="8"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C21" s="8"/>
-      <c r="D21" s="10"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C22" s="8"/>
-      <c r="D22" s="10"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C23" s="8"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C24" s="8"/>
-      <c r="D24" s="10"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C25" s="8"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C26" s="8"/>
-      <c r="D26" s="10"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C27" s="8"/>
-      <c r="D27" s="10"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C29" s="8"/>
-      <c r="D29" s="10"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>